<commit_message>
Atualização página de conjuntura.
</commit_message>
<xml_diff>
--- a/data-raw/Resenhas/resenha-conjuntura.xlsx
+++ b/data-raw/Resenhas/resenha-conjuntura.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>atividadeeconomica</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>setorpublico.es</t>
-  </si>
-  <si>
-    <t>Aqui é a resenha sobre setor público capixaba</t>
   </si>
   <si>
     <t xml:space="preserve">A previsão do mercado financeiro para a queda da economia brasileira este ano foi ajustada de 5,46% para 5,28%. Para o próximo ano, a expectativa é de crescimento de 3,50%, a mesma previsão há 14 semanas consecutivas. Em 2022 e 2023, o mercado financeiro continua a projetar expansão de 2,50% do PIB. &lt;br&gt; O indice de Atividade Economica do Banco Central (IBC-Br) que, com cautela, pode ser utilizado como sinalizador do Produto Interno Bruto (PIB), apresentou avanço de 0,02 por cento em outubro na comparação com o mês anterior, de acordo com dado dessazonalizado divulgado BC. O desempenho foi melhor que a expectativa em pesquisa da Reuters de contração de 0,20 por cento, representando o quinto resultado positivo no ano. </t>
@@ -63,6 +60,12 @@
   </si>
   <si>
     <t>setorpublico.br</t>
+  </si>
+  <si>
+    <t>Aqui é a resenha sobre setor público brasileiro.</t>
+  </si>
+  <si>
+    <t>Aqui é a resenha sobre setor público capixaba.</t>
   </si>
 </sst>
 </file>
@@ -444,7 +447,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,33 +485,33 @@
         <v>8</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="201" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>